<commit_message>
removed term papers from modules/Papers/Student/ folder
</commit_message>
<xml_diff>
--- a/overview.xlsx
+++ b/overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\AKTI\AAAAcreditation\CoursePack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A025504C-A4CA-4070-90CF-BD5198E0622E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17405353-0EA9-4170-BAEC-EDE34CF53A2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -344,22 +344,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -372,6 +360,18 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -738,10 +738,10 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -750,10 +750,10 @@
       <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -765,7 +765,7 @@
       <c r="K5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="M5" s="2" t="s">
@@ -774,7 +774,7 @@
       <c r="N5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="P5" s="25" t="s">
         <v>27</v>
       </c>
       <c r="Q5" s="2" t="s">
@@ -789,16 +789,16 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="23"/>
-      <c r="B6" s="18"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="18"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="17"/>
       <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
@@ -806,18 +806,18 @@
         <v>20</v>
       </c>
       <c r="K6" s="13"/>
-      <c r="L6" s="18"/>
+      <c r="L6" s="17"/>
       <c r="M6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="18" t="s">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="18" t="s">
+      <c r="R6" s="17" t="s">
         <v>30</v>
       </c>
       <c r="S6" s="2" t="s">
@@ -828,8 +828,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="23"/>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="17" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -838,8 +838,8 @@
       <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="18"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="17"/>
       <c r="H7" s="2" t="s">
         <v>14</v>
       </c>
@@ -847,16 +847,16 @@
         <v>20</v>
       </c>
       <c r="K7" s="13"/>
-      <c r="L7" s="18"/>
+      <c r="L7" s="17"/>
       <c r="M7" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P7" s="19"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
       <c r="S7" s="2" t="s">
         <v>33</v>
       </c>
@@ -865,16 +865,16 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" s="23"/>
-      <c r="B8" s="18"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="18"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="17"/>
       <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
@@ -882,7 +882,7 @@
         <v>20</v>
       </c>
       <c r="K8" s="13"/>
-      <c r="L8" s="18" t="s">
+      <c r="L8" s="17" t="s">
         <v>1</v>
       </c>
       <c r="M8" s="2" t="s">
@@ -891,9 +891,9 @@
       <c r="N8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="19"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18" t="s">
+      <c r="P8" s="25"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17" t="s">
         <v>31</v>
       </c>
       <c r="S8" s="2" t="s">
@@ -904,8 +904,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A9" s="23"/>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="17" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -914,8 +914,8 @@
       <c r="D9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="18"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="17"/>
       <c r="H9" s="2" t="s">
         <v>16</v>
       </c>
@@ -923,16 +923,16 @@
         <v>20</v>
       </c>
       <c r="K9" s="13"/>
-      <c r="L9" s="18"/>
+      <c r="L9" s="17"/>
       <c r="M9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="19"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
       <c r="S9" s="2" t="s">
         <v>35</v>
       </c>
@@ -941,16 +941,16 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="23"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="18"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="17"/>
       <c r="H10" s="2" t="s">
         <v>17</v>
       </c>
@@ -958,16 +958,16 @@
         <v>20</v>
       </c>
       <c r="K10" s="13"/>
-      <c r="L10" s="18"/>
+      <c r="L10" s="17"/>
       <c r="M10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
       <c r="S10" s="2" t="s">
         <v>26</v>
       </c>
@@ -976,8 +976,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="23"/>
-      <c r="B11" s="18" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -986,8 +986,8 @@
       <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="18"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="17"/>
       <c r="H11" s="2" t="s">
         <v>18</v>
       </c>
@@ -995,7 +995,7 @@
         <v>20</v>
       </c>
       <c r="K11" s="13"/>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="17" t="s">
         <v>2</v>
       </c>
       <c r="M11" s="2" t="s">
@@ -1004,7 +1004,7 @@
       <c r="N11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P11" s="19"/>
+      <c r="P11" s="25"/>
       <c r="Q11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1019,16 +1019,16 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="23"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="18" t="s">
+      <c r="F12" s="21"/>
+      <c r="G12" s="17" t="s">
         <v>1</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -1038,18 +1038,18 @@
         <v>20</v>
       </c>
       <c r="K12" s="13"/>
-      <c r="L12" s="18"/>
+      <c r="L12" s="17"/>
       <c r="M12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="18" t="s">
+      <c r="P12" s="25"/>
+      <c r="Q12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="18" t="s">
+      <c r="R12" s="17" t="s">
         <v>39</v>
       </c>
       <c r="S12" s="2" t="s">
@@ -1060,8 +1060,8 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="23"/>
-      <c r="B13" s="18" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1070,8 +1070,8 @@
       <c r="D13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="18"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="17"/>
       <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1079,16 +1079,16 @@
         <v>20</v>
       </c>
       <c r="K13" s="13"/>
-      <c r="L13" s="18"/>
+      <c r="L13" s="17"/>
       <c r="M13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="19"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
       <c r="S13" s="2" t="s">
         <v>1</v>
       </c>
@@ -1097,16 +1097,16 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="23"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="17"/>
       <c r="H14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>20</v>
       </c>
       <c r="K14" s="13"/>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="17" t="s">
         <v>3</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -1123,9 +1123,9 @@
       <c r="N14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
       <c r="S14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1134,8 +1134,8 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="23"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1144,8 +1144,8 @@
       <c r="D15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="18"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="17"/>
       <c r="H15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1153,16 +1153,16 @@
         <v>20</v>
       </c>
       <c r="K15" s="13"/>
-      <c r="L15" s="18"/>
+      <c r="L15" s="17"/>
       <c r="M15" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
       <c r="S15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1171,16 +1171,16 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="23"/>
-      <c r="B16" s="18"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="18"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="17"/>
       <c r="H16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1188,16 +1188,16 @@
         <v>20</v>
       </c>
       <c r="K16" s="13"/>
-      <c r="L16" s="18"/>
+      <c r="L16" s="17"/>
       <c r="M16" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P16" s="19"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
       <c r="S16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1206,8 +1206,8 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="23"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1216,8 +1216,8 @@
       <c r="D17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="18"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>20</v>
       </c>
       <c r="K17" s="13"/>
-      <c r="L17" s="18" t="s">
+      <c r="L17" s="17" t="s">
         <v>4</v>
       </c>
       <c r="M17" s="2" t="s">
@@ -1234,9 +1234,9 @@
       <c r="N17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P17" s="19"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
       <c r="S17" s="2" t="s">
         <v>5</v>
       </c>
@@ -1245,16 +1245,16 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="23"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="18"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1262,16 +1262,16 @@
         <v>20</v>
       </c>
       <c r="K18" s="13"/>
-      <c r="L18" s="18"/>
+      <c r="L18" s="17"/>
       <c r="M18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
       <c r="S18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1280,8 +1280,8 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A19" s="23"/>
-      <c r="B19" s="18" t="s">
+      <c r="A19" s="19"/>
+      <c r="B19" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1290,8 +1290,8 @@
       <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="18" t="s">
+      <c r="F19" s="21"/>
+      <c r="G19" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -1301,16 +1301,16 @@
         <v>20</v>
       </c>
       <c r="K19" s="13"/>
-      <c r="L19" s="18"/>
+      <c r="L19" s="17"/>
       <c r="M19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
       <c r="S19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1319,16 +1319,16 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="24"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="18"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>20</v>
       </c>
       <c r="K20" s="13"/>
-      <c r="L20" s="18" t="s">
+      <c r="L20" s="17" t="s">
         <v>5</v>
       </c>
       <c r="M20" s="2" t="s">
@@ -1345,9 +1345,9 @@
       <c r="N20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18" t="s">
+      <c r="P20" s="25"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17" t="s">
         <v>40</v>
       </c>
       <c r="S20" s="2" t="s">
@@ -1358,8 +1358,8 @@
       </c>
     </row>
     <row r="21" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F21" s="25"/>
-      <c r="G21" s="18"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="17"/>
       <c r="H21" s="2" t="s">
         <v>14</v>
       </c>
@@ -1367,16 +1367,16 @@
         <v>20</v>
       </c>
       <c r="K21" s="13"/>
-      <c r="L21" s="18"/>
+      <c r="L21" s="17"/>
       <c r="M21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
       <c r="S21" s="2" t="s">
         <v>1</v>
       </c>
@@ -1391,8 +1391,8 @@
       <c r="C22" s="7">
         <v>16</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="18"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="17"/>
       <c r="H22" s="2" t="s">
         <v>15</v>
       </c>
@@ -1400,16 +1400,16 @@
         <v>20</v>
       </c>
       <c r="K22" s="13"/>
-      <c r="L22" s="18"/>
+      <c r="L22" s="17"/>
       <c r="M22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
       <c r="S22" s="2" t="s">
         <v>2</v>
       </c>
@@ -1424,8 +1424,8 @@
       <c r="C23" s="3">
         <v>56</v>
       </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="18"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="17"/>
       <c r="H23" s="2" t="s">
         <v>16</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>20</v>
       </c>
       <c r="K23" s="13"/>
-      <c r="L23" s="18" t="s">
+      <c r="L23" s="17" t="s">
         <v>6</v>
       </c>
       <c r="M23" s="2" t="s">
@@ -1442,9 +1442,9 @@
       <c r="N23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
       <c r="S23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1459,8 +1459,8 @@
       <c r="C24" s="3">
         <v>26</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="18"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="17"/>
       <c r="H24" s="2" t="s">
         <v>17</v>
       </c>
@@ -1468,16 +1468,16 @@
         <v>20</v>
       </c>
       <c r="K24" s="13"/>
-      <c r="L24" s="18"/>
+      <c r="L24" s="17"/>
       <c r="M24" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P24" s="19"/>
-      <c r="Q24" s="18"/>
-      <c r="R24" s="18"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
       <c r="S24" s="2" t="s">
         <v>4</v>
       </c>
@@ -1492,8 +1492,8 @@
       <c r="C25" s="3">
         <v>25</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="18"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="2" t="s">
         <v>18</v>
       </c>
@@ -1501,16 +1501,16 @@
         <v>20</v>
       </c>
       <c r="K25" s="13"/>
-      <c r="L25" s="18"/>
+      <c r="L25" s="17"/>
       <c r="M25" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="19"/>
-      <c r="Q25" s="18"/>
-      <c r="R25" s="18"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
       <c r="S25" s="2" t="s">
         <v>5</v>
       </c>
@@ -1526,8 +1526,8 @@
         <f>SUM(C22:C25)</f>
         <v>123</v>
       </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="18" t="s">
+      <c r="F26" s="21"/>
+      <c r="G26" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H26" s="2" t="s">
@@ -1537,7 +1537,7 @@
         <v>20</v>
       </c>
       <c r="K26" s="13"/>
-      <c r="L26" s="18" t="s">
+      <c r="L26" s="17" t="s">
         <v>7</v>
       </c>
       <c r="M26" s="2" t="s">
@@ -1546,9 +1546,9 @@
       <c r="N26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P26" s="19"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
       <c r="S26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1557,8 +1557,8 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F27" s="25"/>
-      <c r="G27" s="18"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="17"/>
       <c r="H27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1566,16 +1566,16 @@
         <v>20</v>
       </c>
       <c r="K27" s="13"/>
-      <c r="L27" s="18"/>
+      <c r="L27" s="17"/>
       <c r="M27" s="2" t="s">
         <v>23</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="18"/>
-      <c r="R27" s="18"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
       <c r="S27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1584,8 +1584,8 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F28" s="25"/>
-      <c r="G28" s="18"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="17"/>
       <c r="H28" s="2" t="s">
         <v>14</v>
       </c>
@@ -1593,14 +1593,14 @@
         <v>20</v>
       </c>
       <c r="K28" s="13"/>
-      <c r="L28" s="18"/>
+      <c r="L28" s="17"/>
       <c r="M28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="N28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P28" s="19"/>
+      <c r="P28" s="25"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2" t="s">
@@ -1617,16 +1617,16 @@
       <c r="C29" t="s">
         <v>47</v>
       </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="18"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="17"/>
       <c r="H29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K29" s="17"/>
-      <c r="L29" s="18" t="s">
+      <c r="K29" s="24"/>
+      <c r="L29" s="17" t="s">
         <v>24</v>
       </c>
       <c r="M29" s="6" t="s">
@@ -1635,7 +1635,7 @@
       <c r="N29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P29" s="20"/>
+      <c r="P29" s="26"/>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
       <c r="S29" s="4" t="s">
@@ -1646,16 +1646,16 @@
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F30" s="25"/>
-      <c r="G30" s="18"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="17"/>
       <c r="H30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K30" s="17"/>
-      <c r="L30" s="18"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="17"/>
       <c r="M30" s="6" t="s">
         <v>26</v>
       </c>
@@ -1664,8 +1664,8 @@
       </c>
     </row>
     <row r="31" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F31" s="25"/>
-      <c r="G31" s="18"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="17"/>
       <c r="H31" s="2" t="s">
         <v>17</v>
       </c>
@@ -1673,24 +1673,24 @@
         <v>20</v>
       </c>
       <c r="K31" s="14"/>
-      <c r="L31" s="21"/>
+      <c r="L31" s="18"/>
       <c r="M31" s="4"/>
       <c r="N31" s="5"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="F32" s="25"/>
-      <c r="G32" s="18"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="17"/>
       <c r="H32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L32" s="22"/>
+      <c r="L32" s="23"/>
     </row>
     <row r="33" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F33" s="25"/>
-      <c r="G33" s="18" t="s">
+      <c r="F33" s="21"/>
+      <c r="G33" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H33" s="2" t="s">
@@ -1699,77 +1699,77 @@
       <c r="I33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L33" s="22"/>
+      <c r="L33" s="23"/>
     </row>
     <row r="34" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F34" s="25"/>
-      <c r="G34" s="18"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="17"/>
       <c r="H34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L34" s="22"/>
+      <c r="L34" s="23"/>
     </row>
     <row r="35" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F35" s="25"/>
-      <c r="G35" s="18"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="17"/>
       <c r="H35" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L35" s="22"/>
+      <c r="L35" s="23"/>
     </row>
     <row r="36" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F36" s="25"/>
-      <c r="G36" s="18"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="17"/>
       <c r="H36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L36" s="22"/>
+      <c r="L36" s="23"/>
     </row>
     <row r="37" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F37" s="25"/>
-      <c r="G37" s="18"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="17"/>
       <c r="H37" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L37" s="22"/>
+      <c r="L37" s="23"/>
     </row>
     <row r="38" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F38" s="25"/>
-      <c r="G38" s="18"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="17"/>
       <c r="H38" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L38" s="22"/>
+      <c r="L38" s="23"/>
     </row>
     <row r="39" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F39" s="25"/>
-      <c r="G39" s="18"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="17"/>
       <c r="H39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L39" s="22"/>
+      <c r="L39" s="23"/>
     </row>
     <row r="40" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F40" s="25"/>
-      <c r="G40" s="18" t="s">
+      <c r="F40" s="21"/>
+      <c r="G40" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H40" s="2" t="s">
@@ -1778,11 +1778,11 @@
       <c r="I40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L40" s="22"/>
+      <c r="L40" s="23"/>
     </row>
     <row r="41" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F41" s="25"/>
-      <c r="G41" s="18"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="17"/>
       <c r="H41" s="2" t="s">
         <v>13</v>
       </c>
@@ -1791,8 +1791,8 @@
       </c>
     </row>
     <row r="42" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F42" s="25"/>
-      <c r="G42" s="18"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="17"/>
       <c r="H42" s="2" t="s">
         <v>14</v>
       </c>
@@ -1801,8 +1801,8 @@
       </c>
     </row>
     <row r="43" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F43" s="25"/>
-      <c r="G43" s="18"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="17"/>
       <c r="H43" s="2" t="s">
         <v>15</v>
       </c>
@@ -1811,8 +1811,8 @@
       </c>
     </row>
     <row r="44" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F44" s="25"/>
-      <c r="G44" s="18"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="17"/>
       <c r="H44" s="2" t="s">
         <v>16</v>
       </c>
@@ -1821,8 +1821,8 @@
       </c>
     </row>
     <row r="45" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F45" s="25"/>
-      <c r="G45" s="18"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="17"/>
       <c r="H45" s="2" t="s">
         <v>17</v>
       </c>
@@ -1831,8 +1831,8 @@
       </c>
     </row>
     <row r="46" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F46" s="25"/>
-      <c r="G46" s="18"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="17"/>
       <c r="H46" s="2" t="s">
         <v>18</v>
       </c>
@@ -1841,8 +1841,8 @@
       </c>
     </row>
     <row r="47" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F47" s="25"/>
-      <c r="G47" s="18" t="s">
+      <c r="F47" s="21"/>
+      <c r="G47" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H47" s="2" t="s">
@@ -1853,8 +1853,8 @@
       </c>
     </row>
     <row r="48" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F48" s="25"/>
-      <c r="G48" s="18"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="17"/>
       <c r="H48" s="2" t="s">
         <v>13</v>
       </c>
@@ -1863,8 +1863,8 @@
       </c>
     </row>
     <row r="49" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F49" s="25"/>
-      <c r="G49" s="18"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="17"/>
       <c r="H49" s="2" t="s">
         <v>14</v>
       </c>
@@ -1873,8 +1873,8 @@
       </c>
     </row>
     <row r="50" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F50" s="25"/>
-      <c r="G50" s="18"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="17"/>
       <c r="H50" s="2" t="s">
         <v>15</v>
       </c>
@@ -1883,8 +1883,8 @@
       </c>
     </row>
     <row r="51" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F51" s="25"/>
-      <c r="G51" s="18"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="17"/>
       <c r="H51" s="2" t="s">
         <v>16</v>
       </c>
@@ -1893,8 +1893,8 @@
       </c>
     </row>
     <row r="52" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F52" s="25"/>
-      <c r="G52" s="18"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="17"/>
       <c r="H52" s="2" t="s">
         <v>17</v>
       </c>
@@ -1903,8 +1903,8 @@
       </c>
     </row>
     <row r="53" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F53" s="25"/>
-      <c r="G53" s="18"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="17"/>
       <c r="H53" s="2" t="s">
         <v>18</v>
       </c>
@@ -1913,8 +1913,8 @@
       </c>
     </row>
     <row r="54" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F54" s="25"/>
-      <c r="G54" s="18" t="s">
+      <c r="F54" s="21"/>
+      <c r="G54" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H54" s="2" t="s">
@@ -1925,8 +1925,8 @@
       </c>
     </row>
     <row r="55" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F55" s="25"/>
-      <c r="G55" s="18"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="17"/>
       <c r="H55" s="2" t="s">
         <v>13</v>
       </c>
@@ -1935,8 +1935,8 @@
       </c>
     </row>
     <row r="56" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F56" s="25"/>
-      <c r="G56" s="18"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="17"/>
       <c r="H56" s="2" t="s">
         <v>14</v>
       </c>
@@ -1945,8 +1945,8 @@
       </c>
     </row>
     <row r="57" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F57" s="25"/>
-      <c r="G57" s="18"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="17"/>
       <c r="H57" s="2" t="s">
         <v>15</v>
       </c>
@@ -1955,8 +1955,8 @@
       </c>
     </row>
     <row r="58" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F58" s="25"/>
-      <c r="G58" s="18"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="17"/>
       <c r="H58" s="2" t="s">
         <v>16</v>
       </c>
@@ -1965,8 +1965,8 @@
       </c>
     </row>
     <row r="59" spans="6:11" x14ac:dyDescent="0.35">
-      <c r="F59" s="25"/>
-      <c r="G59" s="18"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="17"/>
       <c r="H59" s="2" t="s">
         <v>17</v>
       </c>
@@ -1975,8 +1975,8 @@
       </c>
     </row>
     <row r="60" spans="6:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F60" s="26"/>
-      <c r="G60" s="21"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="18"/>
       <c r="H60" s="4" t="s">
         <v>18</v>
       </c>
@@ -1990,6 +1990,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="L20:L22"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="Q6:Q10"/>
+    <mergeCell ref="R12:R19"/>
+    <mergeCell ref="R20:R27"/>
+    <mergeCell ref="Q12:Q27"/>
+    <mergeCell ref="P5:P29"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="L26:L28"/>
+    <mergeCell ref="L29:L31"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="L14:L16"/>
+    <mergeCell ref="L17:L19"/>
+    <mergeCell ref="G40:G46"/>
+    <mergeCell ref="G47:G53"/>
+    <mergeCell ref="L32:L34"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="L38:L40"/>
     <mergeCell ref="G54:G60"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="B17:B18"/>
@@ -2006,28 +2028,6 @@
     <mergeCell ref="G19:G25"/>
     <mergeCell ref="G26:G32"/>
     <mergeCell ref="G33:G39"/>
-    <mergeCell ref="G40:G46"/>
-    <mergeCell ref="G47:G53"/>
-    <mergeCell ref="L32:L34"/>
-    <mergeCell ref="L35:L37"/>
-    <mergeCell ref="L38:L40"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="L8:L10"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="L14:L16"/>
-    <mergeCell ref="L17:L19"/>
-    <mergeCell ref="L20:L22"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="Q6:Q10"/>
-    <mergeCell ref="R12:R19"/>
-    <mergeCell ref="R20:R27"/>
-    <mergeCell ref="Q12:Q27"/>
-    <mergeCell ref="P5:P29"/>
-    <mergeCell ref="L23:L25"/>
-    <mergeCell ref="L26:L28"/>
-    <mergeCell ref="L29:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>